<commit_message>
template master and sender master complete,genral setting in prograss
</commit_message>
<xml_diff>
--- a/SMSApplication/bin/Debug/demo sample.xlsx
+++ b/SMSApplication/bin/Debug/demo sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>S.No.</t>
   </si>
@@ -90,13 +90,22 @@
     <t>Active</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -153,16 +162,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +472,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +481,7 @@
     <col min="2" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
@@ -487,7 +499,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -499,7 +511,7 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -537,8 +549,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>3</v>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -549,8 +561,8 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2">
-        <v>40370</v>
+      <c r="F2" s="4">
+        <v>40525</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -581,8 +593,8 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>24</v>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -593,7 +605,7 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>40370</v>
       </c>
       <c r="G3" t="s">
@@ -625,8 +637,8 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
-        <v>4</v>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -637,7 +649,7 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>40370</v>
       </c>
       <c r="G4" t="s">
@@ -667,6 +679,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
master for sms sending
</commit_message>
<xml_diff>
--- a/SMSApplication/bin/Debug/demo sample.xlsx
+++ b/SMSApplication/bin/Debug/demo sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>S.No.</t>
   </si>
@@ -78,9 +78,6 @@
     <t>o+</t>
   </si>
   <si>
-    <t>rf1001</t>
-  </si>
-  <si>
     <t>1 thamarai street</t>
   </si>
   <si>
@@ -90,13 +87,79 @@
     <t>Active</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>ravi</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Michael Smith</t>
+  </si>
+  <si>
+    <t>Emily Johnson</t>
+  </si>
+  <si>
+    <t>David Johnson</t>
+  </si>
+  <si>
+    <t>Alexander Brown</t>
+  </si>
+  <si>
+    <t>Christopher Brown</t>
+  </si>
+  <si>
+    <t>Sophia Wilson</t>
+  </si>
+  <si>
+    <t>Daniel Wilson</t>
+  </si>
+  <si>
+    <t>Olivia Davis</t>
+  </si>
+  <si>
+    <t>James Davis</t>
+  </si>
+  <si>
+    <t>William Taylor</t>
+  </si>
+  <si>
+    <t>Andrew Taylor</t>
+  </si>
+  <si>
+    <t>Ava Anderson</t>
+  </si>
+  <si>
+    <t>Matthew Anderson</t>
+  </si>
+  <si>
+    <t>Noah Clark</t>
+  </si>
+  <si>
+    <t>Benjamin Clark</t>
+  </si>
+  <si>
+    <t>Mia Martinez</t>
+  </si>
+  <si>
+    <t>Joseph Martinez</t>
+  </si>
+  <si>
+    <t>Ethan Rodriguez</t>
+  </si>
+  <si>
+    <t>Anthony Rodriguez</t>
+  </si>
+  <si>
+    <t>V - A</t>
+  </si>
+  <si>
+    <t>VII - A</t>
+  </si>
+  <si>
+    <t>VIII - A</t>
+  </si>
+  <si>
+    <t>VI - A</t>
   </si>
 </sst>
 </file>
@@ -162,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,10 +233,16 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,7 +550,7 @@
     <col min="2" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
@@ -511,7 +580,7 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -549,19 +618,19 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>40525</v>
       </c>
       <c r="G2" t="s">
@@ -573,39 +642,39 @@
       <c r="I2">
         <v>9788492020</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
       </c>
       <c r="O2">
         <v>626001</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3">
         <v>40370</v>
       </c>
       <c r="G3" t="s">
@@ -617,39 +686,39 @@
       <c r="I3">
         <v>9788492020</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3">
+        <v>239</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
       </c>
       <c r="O3">
         <v>626001</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3">
         <v>40370</v>
       </c>
       <c r="G4" t="s">
@@ -661,21 +730,425 @@
       <c r="I4">
         <v>9788492020</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>381</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>21</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
       </c>
       <c r="O4">
         <v>626001</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3">
+        <v>40525</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>9788492002</v>
+      </c>
+      <c r="I5">
+        <v>9788492020</v>
+      </c>
+      <c r="J5">
+        <v>403</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5">
+        <v>626001</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>9788492002</v>
+      </c>
+      <c r="I6">
+        <v>9788492020</v>
+      </c>
+      <c r="J6">
+        <v>424</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6">
+        <v>626001</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>9788492002</v>
+      </c>
+      <c r="I7">
+        <v>9788492020</v>
+      </c>
+      <c r="J7">
+        <v>427</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7">
+        <v>626001</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3">
+        <v>40525</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>9788492002</v>
+      </c>
+      <c r="I8">
+        <v>9788492020</v>
+      </c>
+      <c r="J8">
+        <v>435</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>626001</v>
+      </c>
+      <c r="P8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>9788492002</v>
+      </c>
+      <c r="I9">
+        <v>9788492020</v>
+      </c>
+      <c r="J9">
+        <v>458</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9">
+        <v>626001</v>
+      </c>
+      <c r="P9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>9788492002</v>
+      </c>
+      <c r="I10">
+        <v>9788492020</v>
+      </c>
+      <c r="J10">
+        <v>493</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10">
+        <v>626001</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3">
+        <v>40525</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>9788492002</v>
+      </c>
+      <c r="I11">
+        <v>9788492020</v>
+      </c>
+      <c r="J11">
+        <v>506</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11">
+        <v>626001</v>
+      </c>
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>9788492002</v>
+      </c>
+      <c r="I12">
+        <v>9788492020</v>
+      </c>
+      <c r="J12">
+        <v>516</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12">
+        <v>626001</v>
+      </c>
+      <c r="P12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3">
+        <v>40370</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13">
+        <v>9788492002</v>
+      </c>
+      <c r="I13">
+        <v>9788492020</v>
+      </c>
+      <c r="J13">
+        <v>518</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13">
+        <v>626001</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="C15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>